<commit_message>
Added initiative concept. Started with very basic battle flow.
</commit_message>
<xml_diff>
--- a/Bosses.xlsx
+++ b/Bosses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5618F7-1E44-41AC-90E1-5A935E3F20B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD64B4AB-2443-4AE9-9678-CC9E3EF973F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>SixBoss6</t>
+  </si>
+  <si>
+    <t>Initiative</t>
   </si>
 </sst>
 </file>
@@ -656,9 +659,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G49" totalsRowShown="0">
-  <autoFilter ref="A1:G49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H49" totalsRowShown="0">
+  <autoFilter ref="A1:H49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Id">
       <calculatedColumnFormula>RANDBETWEEN(1000,999999)</calculatedColumnFormula>
     </tableColumn>
@@ -667,6 +670,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="TradeRowSize"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Manna"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="HandSize"/>
+    <tableColumn id="4" xr3:uid="{0DFC22A3-D3C9-4145-832F-73CB56B20BBB}" name="Initiative"/>
     <tableColumn id="3" xr3:uid="{46ACB84A-F66C-4386-9B32-F6C984AE3CC4}" name="Cards"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -970,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,11 +987,11 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="165.7109375" customWidth="1"/>
+    <col min="6" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="165.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1007,10 +1011,13 @@
         <v>11</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1029,11 +1036,14 @@
       <c r="F2">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1052,11 +1062,14 @@
       <c r="F3">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1075,11 +1088,14 @@
       <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1098,11 +1114,14 @@
       <c r="F5">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1121,11 +1140,14 @@
       <c r="F6">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1144,7 +1166,10 @@
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP - battle loop.
</commit_message>
<xml_diff>
--- a/Bosses.xlsx
+++ b/Bosses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD64B4AB-2443-4AE9-9678-CC9E3EF973F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD3CEB3-6EC8-4900-86A0-65D7234B7544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -39,24 +39,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Boss1</t>
-  </si>
-  <si>
-    <t>Boss2</t>
-  </si>
-  <si>
-    <t>Boss3</t>
-  </si>
-  <si>
-    <t>Boss4</t>
-  </si>
-  <si>
-    <t>Boss5</t>
-  </si>
-  <si>
-    <t>Boss6</t>
-  </si>
-  <si>
     <t>Health</t>
   </si>
   <si>
@@ -90,25 +72,40 @@
     <t>Mage1, Mage2, Mage8</t>
   </si>
   <si>
-    <t>AwehBaus1</t>
-  </si>
-  <si>
-    <t>IRBoss2</t>
-  </si>
-  <si>
-    <t>TreeBoss3</t>
-  </si>
-  <si>
-    <t>FoBo4</t>
-  </si>
-  <si>
-    <t>FiveBoss5</t>
-  </si>
-  <si>
-    <t>SixBoss6</t>
-  </si>
-  <si>
     <t>Initiative</t>
+  </si>
+  <si>
+    <t>BossA</t>
+  </si>
+  <si>
+    <t>BossB</t>
+  </si>
+  <si>
+    <t>BossC</t>
+  </si>
+  <si>
+    <t>BossD</t>
+  </si>
+  <si>
+    <t>BossE</t>
+  </si>
+  <si>
+    <t>BossF</t>
+  </si>
+  <si>
+    <t>B_A</t>
+  </si>
+  <si>
+    <t>B_B</t>
+  </si>
+  <si>
+    <t>B_C</t>
+  </si>
+  <si>
+    <t>B_D</t>
+  </si>
+  <si>
+    <t>B_F</t>
   </si>
 </sst>
 </file>
@@ -977,7 +974,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,30 +996,30 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>120</v>
@@ -1040,15 +1037,15 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>150</v>
@@ -1066,15 +1063,15 @@
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>165</v>
@@ -1092,15 +1089,15 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>120</v>
@@ -1118,15 +1115,15 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>95</v>
@@ -1144,15 +1141,15 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>110</v>
@@ -1170,7 +1167,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More refactors to align with new simpler game goals.
</commit_message>
<xml_diff>
--- a/Bosses.xlsx
+++ b/Bosses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD3CEB3-6EC8-4900-86A0-65D7234B7544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:101_{6D53DF05-788F-4C0F-BB56-0CA6E3E32450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9585" yWindow="3675" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosses" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -42,37 +42,7 @@
     <t>Health</t>
   </si>
   <si>
-    <t>TradeRowSize</t>
-  </si>
-  <si>
     <t>Manna</t>
-  </si>
-  <si>
-    <t>HandSize</t>
-  </si>
-  <si>
-    <t>Cards</t>
-  </si>
-  <si>
-    <t>Mage1, Mage2, Mage3</t>
-  </si>
-  <si>
-    <t>Mage1, Mage2, Mage4</t>
-  </si>
-  <si>
-    <t>Mage1, Mage2, Mage5</t>
-  </si>
-  <si>
-    <t>Mage1, Mage2, Mage6</t>
-  </si>
-  <si>
-    <t>Mage1, Mage2, Mage7</t>
-  </si>
-  <si>
-    <t>Mage1, Mage2, Mage8</t>
-  </si>
-  <si>
-    <t>Initiative</t>
   </si>
   <si>
     <t>BossA</t>
@@ -656,28 +626,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H49" totalsRowShown="0">
-  <autoFilter ref="A1:H49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D49" totalsRowShown="0">
+  <autoFilter ref="A1:D49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Id">
       <calculatedColumnFormula>RANDBETWEEN(1000,999999)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Health"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="TradeRowSize"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Manna"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="HandSize"/>
-    <tableColumn id="4" xr3:uid="{0DFC22A3-D3C9-4145-832F-73CB56B20BBB}" name="Initiative"/>
-    <tableColumn id="3" xr3:uid="{46ACB84A-F66C-4386-9B32-F6C984AE3CC4}" name="Cards"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Manna"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -715,7 +681,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -821,7 +787,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -963,7 +929,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -971,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +954,7 @@
     <col min="8" max="8" width="165.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1001,173 +967,89 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
       </c>
       <c r="C2">
         <v>120</v>
       </c>
       <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3">
         <v>150</v>
       </c>
       <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>165</v>
       </c>
       <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>120</v>
       </c>
       <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>95</v>
       </c>
       <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>110</v>
       </c>
       <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
         <v>4</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1177,4 +1059,10 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{aa35b0db-f3d5-44fb-8983-08d6070f3256}" enabled="1" method="Privileged" siteId="{1d90004f-71a2-4f73-8d29-ccfae227b21b}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>